<commit_message>
update tracking + rapport final
</commit_message>
<xml_diff>
--- a/tracking/DARPA_G_Tracking.xlsx
+++ b/tracking/DARPA_G_Tracking.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="146">
   <si>
     <t>Project Information</t>
   </si>
@@ -109,7 +109,7 @@
     <t>Remaining</t>
   </si>
   <si>
-    <t>Progress</t>
+    <t>Progress (%)</t>
   </si>
   <si>
     <t>Delai</t>
@@ -292,6 +292,12 @@
     <t>diff initial - actual</t>
   </si>
   <si>
+    <t>Jours de travail restant</t>
+  </si>
+  <si>
+    <t>Jours de travail manquant</t>
+  </si>
+  <si>
     <t>Tâche</t>
   </si>
   <si>
@@ -394,7 +400,10 @@
     <t>Developpement fonctionnel Anagrammeur</t>
   </si>
   <si>
-    <t>?</t>
+    <t>DWJ</t>
+  </si>
+  <si>
+    <t>Developpement webservice joueur</t>
   </si>
   <si>
     <t>Suivi des tâches, rectification du inital workload</t>
@@ -410,6 +419,36 @@
   </si>
   <si>
     <t>Developpement classes communes : ajout de méthodes dans Plateau et nouvelle classe Placement</t>
+  </si>
+  <si>
+    <t>Developpement fonctionnalités partie</t>
+  </si>
+  <si>
+    <t>Intégration docker toutes classes</t>
+  </si>
+  <si>
+    <t>Web service pour Anagrammeur</t>
+  </si>
+  <si>
+    <t>Développement fonctionnalités joueur : joueur choisi un mot et le place</t>
+  </si>
+  <si>
+    <t>Développement d'une classe pour l'échange avec Partie</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tests fonctionnels pour classe Partie </t>
+  </si>
+  <si>
+    <t>Intégration spring à Joueur</t>
+  </si>
+  <si>
+    <t>Redaction du rapport final de suivi de projet et inscription dans le tracking history</t>
+  </si>
+  <si>
+    <t>Script python</t>
+  </si>
+  <si>
+    <t>?</t>
   </si>
   <si>
     <t>SUM de Workload</t>
@@ -760,7 +799,7 @@
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" invalid="1" refreshOnLoad="1">
   <cacheSource type="worksheet">
-    <worksheetSource ref="C3:H79" sheet="Tracking"/>
+    <worksheetSource ref="C3:H110" sheet="Tracking"/>
   </cacheSource>
   <cacheFields>
     <cacheField name="Date" numFmtId="164">
@@ -774,6 +813,11 @@
         <d v="2022-05-26T00:00:00Z"/>
         <d v="2022-05-30T00:00:00Z"/>
         <d v="2022-05-31T00:00:00Z"/>
+        <d v="2022-06-07T00:00:00Z"/>
+        <d v="2022-06-08T00:00:00Z"/>
+        <d v="2022-06-09T00:00:00Z"/>
+        <d v="2022-06-10T00:00:00Z"/>
+        <d v="2022-06-13T00:00:00Z"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Who" numFmtId="0">
@@ -804,16 +848,26 @@
         <s v="SWS"/>
         <s v="DOCK"/>
         <s v="R"/>
+        <s v="DPWS"/>
+        <s v="DWJ"/>
+        <s v="DANWS"/>
+        <s v="DAWS"/>
+        <s v="DJWS"/>
+        <s v="?"/>
       </sharedItems>
     </cacheField>
-    <cacheField name="Workload" numFmtId="0">
-      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1">
+    <cacheField name="Workload">
+      <sharedItems containsMixedTypes="1" containsNumber="1">
         <n v="0.2"/>
         <n v="0.5"/>
         <n v="0.1"/>
         <n v="0.3"/>
         <n v="1.0"/>
         <n v="1.3"/>
+        <n v="0.25"/>
+        <n v="0.4"/>
+        <n v="0.05"/>
+        <s v="?"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Comment" numFmtId="0">
@@ -838,6 +892,25 @@
         <s v="Suivi de projet, organisation du excel de tracking"/>
         <s v="Développement anagrammeur"/>
         <s v="Diagramme de GANTT, mise à jour du tracking"/>
+        <s v="Tests spring pour Partie"/>
+        <s v="Developpement fonctionnel joueur"/>
+        <s v="Developpement fonctionnel Anagrammeur"/>
+        <s v="Developpement webservice joueur"/>
+        <s v="Suivi des tâches, rectification du inital workload"/>
+        <s v="Developpement web service Anagrammeur"/>
+        <s v="Mise en place Docker pour Anagrammeur"/>
+        <s v="Vidéo de monsieur Renevier"/>
+        <s v="Developpement classes communes : ajout de méthodes dans Plateau et nouvelle classe Placement"/>
+        <s v="Developpement fonctionnalités partie"/>
+        <s v="Intégration docker toutes classes"/>
+        <s v="Web service pour Anagrammeur"/>
+        <s v="Développement fonctionnalités joueur : joueur choisi un mot et le place"/>
+        <s v="Développement d'une classe pour l'échange avec Partie"/>
+        <s v="Tests fonctionnels pour classe Partie "/>
+        <s v="Intégration spring à Joueur"/>
+        <s v="Redaction du rapport final de suivi de projet et inscription dans le tracking history"/>
+        <s v="Script python"/>
+        <s v="?"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Remain" numFmtId="0">
@@ -851,7 +924,7 @@
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tableau croisé dynamique" cacheId="0" dataCaption="" compact="0" compactData="0">
-  <location ref="A1:H19" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <location ref="A1:H25" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields>
     <pivotField name="Date" compact="0" numFmtId="164" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items>
@@ -864,6 +937,11 @@
         <item x="6"/>
         <item x="7"/>
         <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item x="12"/>
+        <item x="13"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -880,17 +958,23 @@
     </pivotField>
     <pivotField name="What" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
       <items>
+        <item x="21"/>
         <item x="2"/>
         <item x="4"/>
         <item x="7"/>
         <item x="12"/>
+        <item x="18"/>
+        <item x="19"/>
         <item x="8"/>
         <item x="9"/>
         <item x="6"/>
         <item x="11"/>
+        <item x="20"/>
         <item x="14"/>
         <item x="5"/>
         <item x="10"/>
+        <item x="16"/>
+        <item x="17"/>
         <item x="3"/>
         <item x="15"/>
         <item x="13"/>
@@ -907,6 +991,10 @@
         <item x="3"/>
         <item x="4"/>
         <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -932,6 +1020,25 @@
         <item x="17"/>
         <item x="18"/>
         <item x="19"/>
+        <item x="20"/>
+        <item x="21"/>
+        <item x="22"/>
+        <item x="23"/>
+        <item x="24"/>
+        <item x="25"/>
+        <item x="26"/>
+        <item x="27"/>
+        <item x="28"/>
+        <item x="29"/>
+        <item x="30"/>
+        <item x="31"/>
+        <item x="32"/>
+        <item x="33"/>
+        <item x="34"/>
+        <item x="35"/>
+        <item x="36"/>
+        <item x="37"/>
+        <item x="38"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -1312,15 +1419,15 @@
       </c>
       <c r="F21" s="7">
         <f>'Tableau croisé dynamique'!H18</f>
-        <v>4.8</v>
+        <v>0.5</v>
       </c>
       <c r="G21" s="7">
         <f t="shared" ref="G21:G23" si="1">E21-F21</f>
-        <v>1.2</v>
+        <v>5.5</v>
       </c>
       <c r="H21" s="7">
         <f t="shared" ref="H21:H23" si="2">F21/E21*100</f>
-        <v>80</v>
+        <v>8.333333333</v>
       </c>
     </row>
     <row r="22">
@@ -1339,15 +1446,15 @@
       </c>
       <c r="F22" s="7">
         <f>'Tableau croisé dynamique'!H15</f>
-        <v>0.6</v>
+        <v>3</v>
       </c>
       <c r="G22" s="7">
         <f t="shared" si="1"/>
-        <v>0.4</v>
+        <v>-2</v>
       </c>
       <c r="H22" s="7">
         <f t="shared" si="2"/>
-        <v>60</v>
+        <v>300</v>
       </c>
     </row>
     <row r="23">
@@ -1366,15 +1473,15 @@
       </c>
       <c r="F23" s="7">
         <f>'Tableau croisé dynamique'!H14</f>
-        <v>0.9</v>
+        <v>0.5</v>
       </c>
       <c r="G23" s="7">
         <f t="shared" si="1"/>
-        <v>3.1</v>
+        <v>3.5</v>
       </c>
       <c r="H23" s="7">
         <f t="shared" si="2"/>
-        <v>22.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="24">
@@ -1417,15 +1524,15 @@
       </c>
       <c r="F26" s="7">
         <f>'Tableau croisé dynamique'!H9</f>
-        <v>0.6</v>
+        <v>0.2</v>
       </c>
       <c r="G26" s="7">
         <f t="shared" ref="G26:G28" si="4">E26-F26</f>
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="H26" s="7">
         <f t="shared" ref="H26:H28" si="5">F26/E26*100</f>
-        <v>60</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27">
@@ -1444,15 +1551,15 @@
       </c>
       <c r="F27" s="7">
         <f>'Tableau croisé dynamique'!H8</f>
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="G27" s="7">
         <f t="shared" si="4"/>
-        <v>3.8</v>
+        <v>4.5</v>
       </c>
       <c r="H27" s="7">
         <f t="shared" si="5"/>
-        <v>24</v>
+        <v>10</v>
       </c>
     </row>
     <row r="28">
@@ -1532,15 +1639,15 @@
       </c>
       <c r="F31" s="7">
         <f>'Tableau croisé dynamique'!H13</f>
-        <v>2</v>
+        <v>3.45</v>
       </c>
       <c r="G31" s="7">
         <f t="shared" si="7"/>
-        <v>3</v>
+        <v>1.55</v>
       </c>
       <c r="H31" s="7">
         <f t="shared" si="8"/>
-        <v>40</v>
+        <v>69</v>
       </c>
     </row>
     <row r="32">
@@ -1675,15 +1782,15 @@
       </c>
       <c r="F38" s="7">
         <f>'Tableau croisé dynamique'!H5</f>
-        <v>0.6</v>
+        <v>3</v>
       </c>
       <c r="G38" s="7">
         <f t="shared" ref="G38:G40" si="13">E38-F38</f>
-        <v>0.4</v>
+        <v>-2</v>
       </c>
       <c r="H38" s="7">
         <f t="shared" ref="H38:H40" si="14">F38/E38*100</f>
-        <v>60</v>
+        <v>300</v>
       </c>
     </row>
     <row r="39">
@@ -1702,15 +1809,15 @@
       </c>
       <c r="F39" s="7">
         <f>'Tableau croisé dynamique'!H6</f>
-        <v>2.4</v>
+        <v>0.6</v>
       </c>
       <c r="G39" s="7">
         <f t="shared" si="13"/>
-        <v>0.6</v>
+        <v>2.4</v>
       </c>
       <c r="H39" s="7">
         <f t="shared" si="14"/>
-        <v>80</v>
+        <v>20</v>
       </c>
     </row>
     <row r="40">
@@ -1764,15 +1871,15 @@
       </c>
       <c r="F42" s="7">
         <f>'Tableau croisé dynamique'!H7</f>
-        <v>0.6</v>
+        <v>2.9</v>
       </c>
       <c r="G42" s="7">
         <f t="shared" ref="G42:G46" si="16">E42-F42</f>
-        <v>0.4</v>
+        <v>-1.9</v>
       </c>
       <c r="H42" s="7">
         <f t="shared" ref="H42:H46" si="17">F42/E42*100</f>
-        <v>60</v>
+        <v>290</v>
       </c>
     </row>
     <row r="43">
@@ -1790,15 +1897,15 @@
       </c>
       <c r="F43" s="7">
         <f>'Tableau croisé dynamique'!H8</f>
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="G43" s="7">
         <f t="shared" si="16"/>
-        <v>1.8</v>
+        <v>2.5</v>
       </c>
       <c r="H43" s="7">
         <f t="shared" si="17"/>
-        <v>40</v>
+        <v>16.66666667</v>
       </c>
     </row>
     <row r="44">
@@ -1816,15 +1923,15 @@
       </c>
       <c r="F44" s="7">
         <f>'Tableau croisé dynamique'!H16</f>
-        <v>5.2</v>
+        <v>0.6</v>
       </c>
       <c r="G44" s="7">
         <f t="shared" si="16"/>
-        <v>0.8</v>
+        <v>5.4</v>
       </c>
       <c r="H44" s="7">
         <f t="shared" si="17"/>
-        <v>86.66666667</v>
+        <v>10</v>
       </c>
     </row>
     <row r="45">
@@ -1843,15 +1950,15 @@
       </c>
       <c r="F45" s="7">
         <f>'Tableau croisé dynamique'!H11</f>
-        <v>2.6</v>
+        <v>1.45</v>
       </c>
       <c r="G45" s="7">
         <f t="shared" si="16"/>
-        <v>0.4</v>
+        <v>1.55</v>
       </c>
       <c r="H45" s="7">
         <f t="shared" si="17"/>
-        <v>86.66666667</v>
+        <v>48.33333333</v>
       </c>
     </row>
     <row r="46">
@@ -1870,15 +1977,15 @@
       </c>
       <c r="F46" s="7">
         <f>'Tableau croisé dynamique'!H17</f>
-        <v>0.2</v>
+        <v>2.5</v>
       </c>
       <c r="G46" s="7">
         <f t="shared" si="16"/>
-        <v>0.8</v>
+        <v>-1.5</v>
       </c>
       <c r="H46" s="7">
         <f t="shared" si="17"/>
-        <v>20</v>
+        <v>250</v>
       </c>
     </row>
     <row r="47">
@@ -1910,15 +2017,15 @@
       </c>
       <c r="F48" s="7">
         <f>'Tableau croisé dynamique'!H3</f>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="G48" s="7">
         <f t="shared" ref="G48:G49" si="19">E48-F48</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H48" s="7">
         <f t="shared" ref="H48:H49" si="20">F48/E48*100</f>
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1981,7 +2088,7 @@
       </c>
       <c r="G52" s="7">
         <f>SUM(G21:G49)</f>
-        <v>29</v>
+        <v>35.2</v>
       </c>
     </row>
     <row r="53">
@@ -1998,6 +2105,24 @@
     <row r="56">
       <c r="B56" s="3" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="B57" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C57" s="3">
+        <f> 2 * 6 * 1</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C58" s="7">
+        <f>G52-C57</f>
+        <v>23.2</v>
       </c>
     </row>
   </sheetData>
@@ -2032,11 +2157,11 @@
   <sheetData>
     <row r="1" ht="29.25" customHeight="1">
       <c r="A1" s="24" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B1" s="24"/>
       <c r="C1" s="24" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="D1" s="25">
         <v>44690.0</v>
@@ -2182,7 +2307,7 @@
     </row>
     <row r="2">
       <c r="A2" s="26" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="27"/>
@@ -3034,7 +3159,7 @@
     </row>
     <row r="18">
       <c r="A18" s="16" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B18" s="16" t="s">
         <v>58</v>
@@ -17167,39 +17292,40 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
+    <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <cols>
-    <col customWidth="1" min="7" max="7" width="69.25"/>
+    <col customWidth="1" min="7" max="7" width="82.25"/>
     <col customWidth="1" min="8" max="8" width="35.5"/>
   </cols>
   <sheetData>
     <row r="2">
       <c r="B2" s="44" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="3">
       <c r="C3" s="3" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="4">
@@ -17216,7 +17342,7 @@
         <v>0.2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5">
@@ -17233,7 +17359,7 @@
         <v>0.2</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6">
@@ -17250,7 +17376,7 @@
         <v>0.2</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7">
@@ -17267,7 +17393,7 @@
         <v>0.2</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8">
@@ -17284,7 +17410,7 @@
         <v>0.2</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9">
@@ -17301,7 +17427,7 @@
         <v>0.2</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10">
@@ -17318,7 +17444,7 @@
         <v>0.2</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="11">
@@ -17335,7 +17461,7 @@
         <v>0.5</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12">
@@ -17352,7 +17478,7 @@
         <v>0.5</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13">
@@ -17369,7 +17495,7 @@
         <v>0.5</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14">
@@ -17386,7 +17512,7 @@
         <v>0.5</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15">
@@ -17403,7 +17529,7 @@
         <v>0.5</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16">
@@ -17420,7 +17546,7 @@
         <v>0.5</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17">
@@ -17437,7 +17563,7 @@
         <v>0.1</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="18">
@@ -17454,7 +17580,7 @@
         <v>0.5</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="19">
@@ -17471,7 +17597,7 @@
         <v>0.5</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="20">
@@ -17488,7 +17614,7 @@
         <v>0.5</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="21">
@@ -17505,7 +17631,7 @@
         <v>0.5</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="22">
@@ -17522,7 +17648,7 @@
         <v>0.5</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23">
@@ -17539,7 +17665,7 @@
         <v>0.5</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="24">
@@ -17556,7 +17682,7 @@
         <v>0.3</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="25">
@@ -17573,7 +17699,7 @@
         <v>0.3</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="26">
@@ -17590,7 +17716,7 @@
         <v>0.3</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="27">
@@ -17607,7 +17733,7 @@
         <v>0.3</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="28">
@@ -17624,7 +17750,7 @@
         <v>0.3</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="29">
@@ -17641,7 +17767,7 @@
         <v>0.3</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30">
@@ -17658,7 +17784,7 @@
         <v>0.1</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="31">
@@ -17675,7 +17801,7 @@
         <v>0.1</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="32">
@@ -17692,7 +17818,7 @@
         <v>0.1</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="33">
@@ -17709,7 +17835,7 @@
         <v>0.1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="34">
@@ -17726,7 +17852,7 @@
         <v>0.1</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35">
@@ -17743,7 +17869,7 @@
         <v>0.1</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36">
@@ -17760,7 +17886,7 @@
         <v>0.2</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37">
@@ -17777,7 +17903,7 @@
         <v>0.2</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="38">
@@ -17794,7 +17920,7 @@
         <v>0.2</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="39">
@@ -17811,7 +17937,7 @@
         <v>0.2</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="40">
@@ -17828,7 +17954,7 @@
         <v>0.2</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="41">
@@ -17845,7 +17971,7 @@
         <v>0.2</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42">
@@ -17862,7 +17988,7 @@
         <v>0.2</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="43">
@@ -17879,7 +18005,7 @@
         <v>0.2</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="44">
@@ -17896,7 +18022,7 @@
         <v>0.2</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="45">
@@ -17913,7 +18039,7 @@
         <v>0.2</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="46">
@@ -17930,7 +18056,7 @@
         <v>0.2</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="47">
@@ -17947,7 +18073,7 @@
         <v>0.2</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="48">
@@ -17964,7 +18090,7 @@
         <v>1.0</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="49">
@@ -17981,7 +18107,7 @@
         <v>1.0</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50">
@@ -17998,7 +18124,7 @@
         <v>1.0</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51">
@@ -18015,7 +18141,7 @@
         <v>1.0</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52">
@@ -18032,7 +18158,7 @@
         <v>1.0</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53">
@@ -18049,7 +18175,7 @@
         <v>1.0</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54">
@@ -18066,7 +18192,7 @@
         <v>0.1</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="55">
@@ -18083,7 +18209,7 @@
         <v>0.2</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="56">
@@ -18100,7 +18226,7 @@
         <v>0.2</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="57">
@@ -18117,7 +18243,7 @@
         <v>0.2</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="58">
@@ -18134,7 +18260,7 @@
         <v>0.2</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="59">
@@ -18151,7 +18277,7 @@
         <v>0.2</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="60">
@@ -18168,7 +18294,7 @@
         <v>0.2</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="61">
@@ -18185,7 +18311,7 @@
         <v>1.3</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="62">
@@ -18202,7 +18328,7 @@
         <v>1.3</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="63">
@@ -18219,7 +18345,7 @@
         <v>1.3</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="64">
@@ -18236,7 +18362,7 @@
         <v>1.3</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="65">
@@ -18253,7 +18379,7 @@
         <v>1.3</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="66">
@@ -18270,7 +18396,7 @@
         <v>1.3</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
     </row>
     <row r="67">
@@ -18287,7 +18413,7 @@
         <v>0.2</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="68">
@@ -18304,7 +18430,7 @@
         <v>0.2</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="69">
@@ -18321,7 +18447,7 @@
         <v>0.2</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
     </row>
     <row r="70">
@@ -18338,7 +18464,7 @@
         <v>0.2</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="71">
@@ -18355,7 +18481,7 @@
         <v>0.2</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="72">
@@ -18372,7 +18498,7 @@
         <v>0.2</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="73">
@@ -18389,7 +18515,7 @@
         <v>0.2</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="74">
@@ -18406,7 +18532,7 @@
         <v>0.2</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="75">
@@ -18423,7 +18549,7 @@
         <v>0.2</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="76">
@@ -18440,7 +18566,7 @@
         <v>0.2</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
     </row>
     <row r="77">
@@ -18457,7 +18583,7 @@
         <v>0.2</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="78">
@@ -18474,7 +18600,7 @@
         <v>0.2</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="79">
@@ -18491,7 +18617,7 @@
         <v>0.5</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
     </row>
     <row r="80">
@@ -18508,7 +18634,7 @@
         <v>0.1</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="81">
@@ -18525,7 +18651,7 @@
         <v>0.5</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="82">
@@ -18542,7 +18668,7 @@
         <v>0.25</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="83">
@@ -18559,7 +18685,7 @@
         <v>0.5</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="84">
@@ -18576,7 +18702,7 @@
         <v>0.25</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="85">
@@ -18587,13 +18713,13 @@
         <v>20</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F85" s="3" t="s">
-        <v>125</v>
+        <v>53</v>
+      </c>
+      <c r="F85" s="3">
+        <v>0.4</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="86">
@@ -18601,16 +18727,16 @@
         <v>44719.0</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>36</v>
+        <v>127</v>
       </c>
       <c r="F86" s="3">
         <v>0.1</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
     </row>
     <row r="87">
@@ -18618,16 +18744,16 @@
         <v>44719.0</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>69</v>
+        <v>36</v>
       </c>
       <c r="F87" s="3">
-        <v>0.25</v>
+        <v>0.1</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88">
@@ -18635,7 +18761,7 @@
         <v>44719.0</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>69</v>
@@ -18643,8 +18769,8 @@
       <c r="F88" s="3">
         <v>0.25</v>
       </c>
-      <c r="G88" s="45" t="s">
-        <v>127</v>
+      <c r="G88" s="3" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="89">
@@ -18652,16 +18778,16 @@
         <v>44719.0</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
       <c r="F89" s="3">
-        <v>0.1</v>
-      </c>
-      <c r="G89" s="3" t="s">
-        <v>128</v>
+        <v>0.25</v>
+      </c>
+      <c r="G89" s="45" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="90">
@@ -18669,7 +18795,7 @@
         <v>44719.0</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="E90" s="3" t="s">
         <v>79</v>
@@ -18678,49 +18804,49 @@
         <v>0.1</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
     </row>
     <row r="91">
-      <c r="C91" s="46">
+      <c r="C91" s="23">
         <v>44719.0</v>
       </c>
-      <c r="D91" s="36" t="s">
+      <c r="D91" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F91" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G91" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="C92" s="46">
+        <v>44719.0</v>
+      </c>
+      <c r="D92" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="E91" s="3" t="s">
+      <c r="E92" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F91" s="3">
+      <c r="F92" s="3">
         <v>0.2</v>
       </c>
-      <c r="G91" s="3" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="92">
-      <c r="C92" s="23">
-        <v>44719.0</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E92" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F92" s="3">
-        <v>0.1</v>
-      </c>
       <c r="G92" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="93">
       <c r="C93" s="23">
-        <v>44720.0</v>
+        <v>44719.0</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="E93" s="3" t="s">
         <v>75</v>
@@ -18729,10 +18855,319 @@
         <v>0.1</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>130</v>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="94">
+      <c r="C94" s="23">
+        <v>44720.0</v>
+      </c>
+      <c r="D94" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F94" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G94" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="C95" s="23">
+        <v>44721.0</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F95" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G95" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="C96" s="23">
+        <v>44721.0</v>
+      </c>
+      <c r="D96" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F96" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G96" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="C97" s="23">
+        <v>44721.0</v>
+      </c>
+      <c r="D97" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F97" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G97" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="98">
+      <c r="C98" s="23">
+        <v>44721.0</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F98" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="99">
+      <c r="C99" s="23">
+        <v>44721.0</v>
+      </c>
+      <c r="D99" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="F99" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="G99" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="100">
+      <c r="C100" s="23">
+        <v>44722.0</v>
+      </c>
+      <c r="D100" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F100" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="101">
+      <c r="C101" s="23">
+        <v>44722.0</v>
+      </c>
+      <c r="D101" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F101" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G101" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="102">
+      <c r="C102" s="23">
+        <v>44722.0</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E102" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F102" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="103">
+      <c r="C103" s="23">
+        <v>44722.0</v>
+      </c>
+      <c r="D103" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E103" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F103" s="3">
+        <v>0.05</v>
+      </c>
+      <c r="G103" s="3" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="104">
+      <c r="C104" s="23">
+        <v>44722.0</v>
+      </c>
+      <c r="D104" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="F104" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="105">
+      <c r="C105" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="F105" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="G105" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="106">
+      <c r="C106" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D106" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F106" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="G106" s="3" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="107">
+      <c r="C107" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D107" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F107" s="3">
+        <v>0.2</v>
+      </c>
+      <c r="G107" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="108">
+      <c r="C108" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D108" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G108" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="109">
+      <c r="C109" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F109" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G109" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="110">
+      <c r="C110" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F110" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="111">
+      <c r="C111" s="23">
+        <v>44725.0</v>
+      </c>
+      <c r="D111" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="F111" s="3" t="s">
+        <v>143</v>
+      </c>
+      <c r="G111" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>
+  <printOptions gridLines="1" horizontalCentered="1"/>
+  <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup fitToHeight="0" paperSize="9" cellComments="atEnd" orientation="landscape" pageOrder="overThenDown"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -18766,6 +19201,12 @@
     <row r="17"/>
     <row r="18"/>
     <row r="19"/>
+    <row r="20"/>
+    <row r="21"/>
+    <row r="22"/>
+    <row r="23"/>
+    <row r="24"/>
+    <row r="25"/>
   </sheetData>
   <drawing r:id="rId2"/>
 </worksheet>

</xml_diff>